<commit_message>
Get daily reddit data: Tue Apr  2 08:08:01 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_07.xlsx
+++ b/data/2024_04_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C434"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2267 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1btrhho</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Purple rain ☔️</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btrhho</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1btpo0t</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Finally got the gel ombre down</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/birdr3ltszrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1bto86p</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Nail party</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bto86p/nail_party/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1btn1tn</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Top coats</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1btn1tn/top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1btmktw</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>🍓Spring Nails 🍓- This is my second attempt doing someone else’s nails! Lots to improve on but I’m excited!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btmktw</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1btmah5</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Got my nails done for the 3rd time ever, got little strawbs 🍓</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btmah5</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1btm0t9</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>black or white toes ? i will always choose blackkk!!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btm0t9</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1btlte6</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>First set on someone other then myself. Looking for tips to improve and opinions on the nails!</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcruwp2mvyrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1btksaq</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Cateye + chrome nails</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btksaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1btkbx1</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Another “which shape” post. Which do you think looks best?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btkbx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1btjvjq</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Acrylics came off to find this. I assume the red line (and yes it’s indented not just red) is from something they did wrong when they applied the acrylics? Most of them are ok other than looking bad and being indented, but a couple of them don’t feel good. (both hands are like this)</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6robomnogyrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1btjf0o</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>3 day old gel mani🩷</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yy0p5ja9dyrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1btjcjy</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Mooncat mani</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btjcjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1btifje</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>I heard you guys like nails</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/345m4je36yrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1btidd4</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>I've been a lifelong nail-biter. Recently broke the habit, and I am trying to keep my nails looking nice. (Any tips or advice are appreciated, as I am new to this.)</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p447hf2t5yrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1btgzj8</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Last couple of nail art designs + nail growth progress!!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjcm3te1wxrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1btfx1o</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Best at Home Nail Kit for Dipping Powder</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1btfx1o/best_at_home_nail_kit_for_dipping_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1btfpyd</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Swipe right to see how my nails looked when I started BIAB in Sept '23 🥹</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btfpyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1btfbwa</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jm1lnidxkxrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1bta10k</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>I want to try going to a nail salon for the first time but don't know how these things go.</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bta10k/i_want_to_try_going_to_a_nail_salon_for_the_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1bt9pb7</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Help me decide if I love or hate this</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt9pb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1bt84rk</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Nail growth/builder gel</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt84rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1bt7okh</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Best polish to cover nails without bringing attention to nails?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bt7okh/best_polish_to_cover_nails_without_bringing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1bt26ev</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evvfwp901vrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1btemsc</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Red Tulip Nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btemsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1bteln8</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>New set 🥰</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inrujcc5gxrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1bteeiq</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Pastel flower spring nails</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bteeiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1btea4p</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Spring is here 🌷</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btea4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1bte727</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>What do you think of my work?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6q3iy40gdxrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1btdzux</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wreh7x08cxrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1btdw88</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Cat eye frenchies with kisses 💋</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btdw88</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1btdi43</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btdi43</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1btde75</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>The Walmart sets have been perfection lately ✨ (just wish they weren’t so flimsy for us working girlies)</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh4g51ha8xrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1btd6gb</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Just finished painting Cosmo &amp; Wanda Aquarium nails from Fairly odd parents 🤗 took so long omg</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2srtqgmv6xrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1btd4gy</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Made my Own Press ons🤍🌼</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btd4gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1btd21k</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>need help with polygel</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1btd21k/need_help_with_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1btcxm7</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>first time doing press-ons - how did i do?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btcxm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1btcv68</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>spring (accidental) freestyle set!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btcv68</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1btciz2</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>encapsulation will always be my favorite process!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btciz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1btchj0</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>my custom glow in the dark mix on my nail bestie!</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btchj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1btcgdq</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>team red or blue? 🫶</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btcgdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1btcfis</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>the fresh file feeling is unmatcheddd</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btcfis</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1btce8y</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>can’t get enough of this minimal vibe. !</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btce8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1btcd1h</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>cyber butterfly nails</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btcd1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1btcc8u</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>process shots! i really love the blue jelly</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btcc8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1btc8ip</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>blank canvas</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btc8ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1btc7s6</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">some abstract fun blobs! </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0v7ihii0xrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1btbnjn</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>touching up nail polish?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gadado4kwwrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1btbgtk</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Love me some freshies 🤍</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wekg7lddvwrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1btbbay</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpaexynbuwrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1btayd4</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btayd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1btatrj</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>I’m fall in love 😍</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kk9rktu2rwrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1btahd2</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Opal nails 🩵</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btahd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1bt9qms</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Frog Nails!</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt9qms</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1bt9pcy</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Nails that I can wear for just a few hours every day? And take off in the evening?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bt9pcy/nails_that_i_can_wear_for_just_a_few_hours_every/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1bt8yk5</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>I'm seeking the best Dotting Pens and Painting Brushes to gift my partner, who is considering the product I linked. There must be something better than this generic product. She's new to the polishing world. (No set budget.)</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/dp/B08ZSN22HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1bt8g3z</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Redone Finally</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt8g3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1bt7cw6</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Can't stop staring, That color shift is unreal!</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt7cw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1bt78er</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Back at it again with the dots... w/ silver tips 🎭🩶</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bxfsv4qy2wrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1bt608p</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>DIY gel ex rose gold french</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt608p</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1bt4txq</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Shimmery pink almond french tips:)</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt4txq</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1bt4s74</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>DND Inky Point</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt4s74</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1bt49ix</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>My nail tech never misses a beat💅🏽🌸</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt49ix</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1bt44jw</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Been Doing my Partners Nails for years.. Stepped up to Gelly Tips and Gels! So happy with progress!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt44jw</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1bt08ag</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Straight men that paint your nails, what colours do you do?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bt08ag/straight_men_that_paint_your_nails_what_colours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1bt05yp</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted something "girly" and glittery this time </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wa7k7tkshurc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1bszkk4</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>My nail tech is absolutely amazing</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk3vfdtsburc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1bsyctk</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Peel-off nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5u3rhetmxtrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1btt7am</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>First time posting here with my favourite colour</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btt7am</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1btrydb</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>First time!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btrydb/first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1btquzl</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Springy Easter-ish Nails</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cox4s6bb50sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1btqu7h</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btqu7h/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1btnbui</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Howl’s Moving Castle Mystery - Star children</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btnbui</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1btnbgx</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>First thermal. I’m like a child.</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ipk1veqx7zrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1btn92f</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Should I buy an extra bottle of a favorite nail polish?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btn92f/should_i_buy_an_extra_bottle_of_a_favorite_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1btn4me</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>lumen skittle.... lumttle?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btn4me</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1btn028</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do I ask for at a nail salon for this gorgeous color?! I showed a tech this pic and my nails came out looking like a regular sheer pink. Pic from @SetsbySenia on IG. </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozxeg9uc5zrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1btmilu</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Feeling fruity</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btmilu</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1btmev2</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>howl's moving castle mysteries!</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btmev2</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1btlu4j</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Needing some advice</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btlu4j/needing_some_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1btljqo</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Enchanted Polish Holiday 2015</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btljqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1btjbcm</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Springtime strawberry jam vibes (thermal)</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btjbcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1btizx4</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Please help me dupe this, it has been haunting me for months</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btizx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1btiogv</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>absolutely obsessed with mooncat's mermaid bait</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btiogv</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1btioa4</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>going to be teaching my students about odysseus' journey to the underworld tomorrow, so i thought i'd throw on house of hades to match 💙</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btioa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1btijm8</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Top coat stringy</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btijm8/top_coat_stringy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1bthnge</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Heaven help me!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7a97dzm0yrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1bthhf8</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Do you throw test swatches away?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bthhf8/do_you_throw_test_swatches_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1btfke1</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Y’all already know who it is</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btfke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1btfhfa</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Need Recommendations...like bad</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btfhfa/need_recommendationslike_bad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1btesb7</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>newbie wants color suggestions please</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btesb7/newbie_wants_color_suggestions_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1bt8hfp</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt8hfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1btf0ny</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Blue shimmer skittle ✨️🦋</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btf0ny</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1btenrf</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Bubbling out the wazoo</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8enfszjgxrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1bsyxmu</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>same color, different lighting</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bsyxmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1btekki</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Spring time lavender and sage inspo</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqanckjyfxrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1btegq4</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>So juicy &amp; sparkly!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kwdk6oafxrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1bte9wx</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Spent 2+ hours on spring nails instead of spring cleaning 😅</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bte9wx</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1btcjtx</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manucurist LED lamp </t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btcjtx/manucurist_led_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1btcfud</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>One month of wear with regular polish! A realistic look</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btcfud</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1btc881</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>[Polish] Queen of the Dead + The Alchemist</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpdu1cul0xrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1btc2se</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’d consider myself past a “beginner” with gel/gel x extensions. What are products tools that are worth investing in? </t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btc2se/id_consider_myself_past_a_beginner_with_gelgel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1btbnqo</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btbnqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1btajh0</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Beautometry unresponsive?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btajh0/beautometry_unresponsive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1btadpj</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Swatch: "Rhiannon" by Loud</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btadpj/swatch_rhiannon_by_loud/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1bta5ap</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>How to fix a manicure without going back to the salon</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bta5ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1bt7wuj</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Blooming Azalea</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1hdjh8j7wrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1bt7ve5</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>How do you stop obsessive cuticle picking? (ft. ilnp prancer)</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol32guy57wrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1bt7ql8</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>New OPI Infinite Shine Formula with Old Top &amp; Base Coats</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bt7ql8/new_opi_infinite_shine_formula_with_old_top_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1bt5v7t</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Regular polish over gel polish</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bt5v7t/regular_polish_over_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1bt3ctn</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>March 2024 - Manicure Round Up!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt3ctn</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1bt36r8</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>What do magnetic polishes look like without the magnet?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bt36r8/what_do_magnetic_polishes_look_like_without_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1bt1xuw</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The absolute best red combo I have at the minute. </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqs8r71zyurc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1bt0gok</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Easter mani 🐇</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqkqh5evkurc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1bszq1i</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bszq1i/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1bszpee</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bszpee/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1bszp1z</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bszp1z/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1bts0o2</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Idea help</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1bts0o2/idea_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1btrsog</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hihi ♡︎♡︎♡︎ </t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4h6p1azf0sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1btre0n</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>took a shot doing a mcbling set 💖</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpv73dg6b0sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1btrdvq</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my quick simple nails 💅 💕 😍 </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hh92dhg3b0sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1btm6wd</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Prom nails ❄️</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09mvsmlpyyrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1bthwnz</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>I’m a little late because I was sick but this is my Easter set</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m139gmbi2yrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1bte1j9</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Sometimes stickers are the best 💋</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bte1j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1btd4ww</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Just finished painting Cosmo &amp; Wanda Aquarium nails from Fairly odd parents 🤗 took so long omg</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rx9qgfhl6xrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1bt8qep</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Total beginner so it's simple AF but I'm happy with them</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pas1bk2dwrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1bt87ag</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Plaid yellow + green</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh07cx9l9wrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1bt4qhk</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>What do you think about this design? 🤍</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2yii8cjlvrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1bt4f28</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Spring marble gel 🌷</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt4f28</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1bt3ydd</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Another One</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bt3ydd</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1bt0ddo</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Just tried a new design please share your thoughts</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1bt0ddo/just_tried_a_new_design_please_share_your_thoughts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1bt0225</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made a set for my sister </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt0ksp3rgurc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1bszets</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Attempted to do my own nails</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bszets</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr  3 08:08:29 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_07.xlsx
+++ b/data/2024_04_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C434"/>
+  <dimension ref="A1:C601"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7811,6 +7811,2845 @@
         </is>
       </c>
     </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1bum1js</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Anybody scratch their phone with their nails?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bum1js/anybody_scratch_their_phone_with_their_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1bulvue</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>How often do you try something new?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wmn6mr0n7sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1bulo1a</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>We match!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bulo1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1bukttc</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Easter nails with bunny charm </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j966msd7b7sc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1bukqy9</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Press ons 💟</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qob89agba7sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1bue8kq</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Black metal band font inspired nails with a spiral accent.</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bue8kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1bucyqn</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Nail on ring finger broke less than 3 weeks before wedding. Help?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mm0vxlvge5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1bujh83</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Starry Nails!</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bujh83</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1buj236</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my next weird set lolll, the blue acrylic glows in the dark </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/885lzqp6t6sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1buimzc</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Gel Tips By Mee</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecj9gf65p6sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1buhsxy</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>This week's spring nails</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgmb8gyth6sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1bugour</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Clean Mani</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewjl4ug786sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1bug7wz</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Milky white for spring</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bug7wz</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1bufvh5</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>I did my own nails for the 3rd time</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fupay32g16sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1bufaeu</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Tried something new</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vek1gptlw5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1buf9o2</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Pearly set I did this past weekend ✨</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tjvl2q09w5sc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1buf73e</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Tried this stunning blue today 💙</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4j0f1ntv5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1buf6jf</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Love me some press-ons 💕💕</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buf6jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1buf1xc</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buf1xc</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1buc7eh</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>I love my Nail Tech</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buc7eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1bue17c</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons lifting </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bue17c/press_ons_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1budsr7</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>First attempt at pedicure and french tips! If you have any pedicure tips plz let me know!</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1budsr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1buds8l</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Springtime nails!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oir1yzxgk5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1budqlm</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>❤️✨🖤</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a92swdg6k5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1bud6kf</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bud6kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1buczkk</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Feeling fruity</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buczkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1bucxen</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>The MM mix</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l652qeq6e5sc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1bucdtx</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had to do the Hailey nails one time </t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw7n5ot2a5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1buc251</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Broken nails</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1buc251/broken_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1bub724</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Nail inspo</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bub724/nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1bub2zq</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Going to a wedding and can’t decide on a nail color to go with this dress</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t78538n05sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1bubxcv</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Ok I love these 🩷</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bubxcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1bubx0z</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Nails I just finished</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bubx0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1bu90nu</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Shaping Help</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu90nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1bu71ie</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>nails always peel</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02v8wa0l64sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1bu5ox6</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Lil mix-and-match!</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mn77htsfx3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1bu3zu8</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Shape ideas</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu3zu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1bu33g2</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Help!! How to apply press on without white glue spots?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu33g2</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1bubnf1</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Kiss press ons 'West Coast' :3</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fjk0j67q45sc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1bubeb4</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>found a new nail salon and they are AMAZING!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bubeb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1bub9uj</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Engagement/Proposal Nails💍💅🏻</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qh02p7225sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1bub8ly</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Just wanted to show someone my pretty long nails before they break</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0xeggdus15sc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1bub7mz</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Fills always make me feel brand new.</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56bt8zvl15sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1bual9r</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>What do you guys think? ✨️</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bual9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1buacsg</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Would I be right with the assumption that, if I want beautiful long-lasting false nails, I have to have the most dry, rough, [unhealthy] natural nails underneath? Is it possible to have healthy strong natural nails upon removal of fake ones? Or are they a commitment?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1buacsg/would_i_be_right_with_the_assumption_that_if_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1bua8e2</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Free hand lines!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bua8e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1bua87u</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Advice on nail breakage</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bua87u/advice_on_nail_breakage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1bua1p0</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>miami vibes</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48kcbkk7t4sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1bu98ba</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>APRILS SET OF NAILS 40$ I'm debating on painting the 2 middle with glitter..... hmm what to do what to do. Leave as is, or glitter the 2?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu98ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1bu92i6</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>First post: Spyro nails (: 🎮</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu92i6</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1bu8skk</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Embedded Flower Nails!!!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu8skk</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1bu8m2v</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Colour Club's copper holo is so stunning</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72uky5fgh4sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1bu84tl</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>What is the best option for me?</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bu84tl/what_is_the_best_option_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1bu7hrs</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Glitter/Confetti French Nails on short Nails</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu7hrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1bu6nrw</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>I think they are precious 😍</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud7cbj1044sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1bu68ln</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>What can I do to fix my nail length/shape situation?</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0alcps8614sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1bu65cn</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Started using rubber base coat to keep my nails protected and they’ve grown out so well!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5m5xlfk04sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1bu5u39</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>First set after taking a break💖</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu5u39</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1bu5mvo</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Spring Vibes! Not my best work but, I'm getting better!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu5mvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1bu5m7g</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic nails consistently lifting </t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zixfte4vw3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1bu4rhb</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>shorties</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu4rhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1bu4k5o</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>DIY gel 🐣</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu4k5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1bu4eo3</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Monomer recs?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bu4eo3/monomer_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1bu3yyp</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>A fun set i did last night! 🎱🍒💕</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu3yyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1bu3hv5</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>CHROME X CATEYE</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu3hv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1bu3gol</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>my friend did my nails</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8x7m8vbqh3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1bu3c2v</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Did my nail tech do a bad job?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu3c2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1bu3126</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>This sub was surprisingly split on almond vs square on me so we’re rolling with coffin ⚰️</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p296pike3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1bu0cmw</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>"Gel Powder" vs "Gel Liquid" vs. "Hard Gel?"</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bu0cmw/gel_powder_vs_gel_liquid_vs_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1btwjjo</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Nail Emergency</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/no7siywdz1sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1bu26xl</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Love this aesthetic</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtfex7sj83sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1bu248q</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Absolutely loving this red orange color ❤️</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu248q</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1btrwfi</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>First timer!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1btrwfi/first_timer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1btooiv</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Help what do I do?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3mu69ctjzrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1btnr06</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Is glamnetic a good company? Is the glue good?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1btnr06/is_glamnetic_a_good_company_is_the_glue_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1bu1t2x</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>what should i do with my nails?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpttueit53sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1bu19rz</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Tortoise nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wz2g478y13sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1bu0uc1</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Spring ready with this set! My hands are really dry rn, brb while I put my oil on 😅</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu0uc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1bu0m2v</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>This week's simple set</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16f5f4a6x2sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1bu0ftn</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Aura nails!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrwk8qltv2sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1btzc7v</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Spontaneous walk in spring set</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffil72v8n2sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1btz5hk</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>solar eclipse nails on myself, 6 hours later and I am READY</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btz5hk</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1btz2cg</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Nails and snow</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9busz35al2sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1btymnc</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Longest set I’ve done!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4g91dlth2sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1btxonc</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>First at home Gel X</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btxonc</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1btxjav</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>❤️🩶❤️</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btxjav</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1btx7b9</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Might be my best work so far!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btx7b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1btx00n</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Issue with nails on one hand</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0z6aqv3p32sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1btwkf4</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My current obsession: short volume nail </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kuaqwb7mz1sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1btwivt</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Red and black smokey nails</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btwivt</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1btw3u5</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Gel-x extensions: Are they worth it? Pls help this natural nail gel girl get her head around it.</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1btw3u5/gelx_extensions_are_they_worth_it_pls_help_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1btujai</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Magnetic polish always amazes me</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4d00o8spd1sc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1btuj97</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>As a male what can I do to make my nails nice and pretty? I only clip and file but they look so bad :(</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btuj97</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1btu9yp</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Second Attempt</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btu9yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1bttq3p</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Do you like french manicure?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed7l6o2j31sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1btti9h</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>🩵🩵🩵</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btti9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1bttb8r</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Love these 🥰</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojsgsebiy0sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1btt9js</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Birthday nails🥹</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btt9js</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1bum933</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Mooncat sales?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bum933/mooncat_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1buhofy</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>HT Life In Plastic + Linear Holo Taco</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buhofy</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1bufu8x</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Acrilate/cyanocrilate allergy</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bufu8x/acrilatecyanocrilate_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1bujhk0</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>🥚Bespeckled Skittle🥚</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bujhk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1buj90m</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Artdone 16 Jars Chrome Nail Powder Nail Art #4 with base Beetles Jelly Gel Nail Polish Neutral Sheer Milky White on almond Gel-x tips</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he38qrowu6sc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1buj2qs</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Mooncat Queen of the Dead and preventing staining - gifts for a friend.</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1buj2qs/mooncat_queen_of_the_dead_and_preventing_staining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1buigb6</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Perfect Blue Holo</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1buigb6/perfect_blue_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1buh0dr</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Underwater hotel room manicure</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rfciq5lxa6sc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1bugya6</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Mom bought press ons and asked me to install them. We both got matching mani’s out of it</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7qhcc3ga6sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1bugjeb</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Do I need to apply a base coat with this?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nse2mecy66sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1bug424</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>ILNP - Rosewater</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65ivgrxe36sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1bufty0</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>tips needed for a beginner lacquerista!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bufty0</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1bufmqd</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Looking for suggestions on a dupe of China Glaze's "Frosty".</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bufmqd/looking_for_suggestions_on_a_dupe_of_china_glazes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1bufky8</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Cirque Georgette color discrepancy</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bufky8</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1buffiy</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Help fixing nails</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58u8zctrx5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1buf9va</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Second attempt at some flowers</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buf9va</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1buf9bv</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Polish that looks like this by itself?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcxmozxcw5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1buetyh</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>DIY Not Today Satan from Venus Fly Trap + Fake Halo</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrus5xhus5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1bueqhr</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Tactical Assault Possum by LynB</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bueqhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1budvxx</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Gel manicure advice please!</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1budvxx/gel_manicure_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1budjdi</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Just got Queen of the Dead</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vz3g43oi5sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1budg26</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Tucking Myself In</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7g2l7qjzh5sc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1bucwmf</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Don't know what to title this 🫠</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6viy89n0e5sc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1buco41</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Rainbow for Spring</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buco41</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1bu9vi8</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>FOTM vs Popcorn &amp; Pjs</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu9vi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1bu9uhm</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Lazy eclipse nails</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0i1akerr4sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1bu9nes</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>The Great Lynx from LynN designs</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu9nes</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1bu8g9l</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Can I get BIAB gel over broken nail?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kytmcfrdg4sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1bu78lo</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Abstract Monarch Butterfly 🦋</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu78lo</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1bu63xw</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let's talk about Toenails </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bu63xw/lets_talk_about_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1bu76rh</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>X-post from r/funny. Yall I am on the floor 🤣</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/funny/s/kkv8XqoVxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1bu6uv4</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Glazed donuts</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu6uv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1bu5zus</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Bye hard gel overlays back to diy manis with dazzle dry</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8vlihljz3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1bu5xu8</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>March Manis- working through my untrieds, plus some old favs</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu5xu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1bu5nl9</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Experience with Krisable Designs polish?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bu5nl9/experience_with_krisable_designs_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1bu55z0</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Help me find a polish :)</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpw69t4st3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1bu4kgp</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Ethereal Snow Globe mysteries spoiler</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r1z1jzyjp3sc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1bu4jym</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Quiet</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu4jym</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1bu3tt2</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>What do I tell the tech If I want these nails</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bu3tt2/what_do_i_tell_the_tech_if_i_want_these_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1bu3p5j</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Shifty magnetics</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu3p5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1bu2vad</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Feeling cute</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1n3u8eed3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1bu11ch</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>What polish is this?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bu11ch/what_polish_is_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1bu0kn9</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>I love ombre nails. I hate ombre nails</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zim484vtw2sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1bu0hyc</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>{PR} Velvety 😍</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npthmi5aw2sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1bu0em8</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Do blurring (tinted) basecoats stain??</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bu0em8/do_blurring_tinted_basecoats_stain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1bu0bzq</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Strangeberry dupe?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bu0bzq/strangeberry_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1bu07tb</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Spring florals to bikini bottom 🌺</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu07tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1btz162</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>6 hours later and I am ready for the solar eclipse!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btz162</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1btyr5x</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Some belated egg candies for Easter 🐣🥚</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbzur8aui2sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1btxm2l</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Favorite Unicorn Pee polish that is still available?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1btxm2l/favorite_unicorn_pee_polish_that_is_still/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1btuk1j</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Received my first ilnp order! And tried to shape my nails for the first time 😅</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btuk1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1bttz2f</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>I feel so shiny</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4aic27ry61sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1btt8jo</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Birthday nails 🥹</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btt8jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1bumw4r</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Easter Nails</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/geb1mxogz7sc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1bulyc5</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>..</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iekyt1r1o7sc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1bulk33</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I went insane </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xne770zbj7sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1bul7f3</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Just finished painting Melanie Martinez inspired nails for my tiktok 🥹 Loved her since I was 11 so happy with this set 😍</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amwg976hf7sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1buj001</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Gel Tips By Me ✨</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5qgpesms6sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1bugie2</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Cute Free-Hand Design? No. Floop's Fooglies? Yes.</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo05ectp66sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1bug70v</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>3d nails</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bug70v</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1bubvy8</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Just finished these</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bubvy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1bu66jz</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Nana nails🎀🖤</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrlgr9yr04sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1bu504a</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>☀️☀️☀️</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sco602pms3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1bu40g3</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>red or black?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu40g3</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1bu3ddu</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Wish I can do this on someone😫</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rle0q4i1h3sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1bu37kv</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Delftware Nails</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bu37kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1bty1a0</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Rococo inspired nails</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bty1a0</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1btx21z</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Blue or Red?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1btx21z</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1btt8sm</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Little fairy land</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fncwotirx0sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Apr  4 08:08:37 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_07.xlsx
+++ b/data/2024_04_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C601"/>
+  <dimension ref="A1:C735"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10650,6 +10650,2284 @@
         </is>
       </c>
     </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1bvgzc6</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Preparing for vocational school next week</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m83subw7yesc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1bvgkhv</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Where to buy nail polish the same colors as these?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bf7ikl2ctesc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1bvfwak</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/poxwo2vclesc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1bvfe14</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>C curve makes some nails look thinner and lopsided on free edge</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bvfe14/c_curve_makes_some_nails_look_thinner_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1bvezuc</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>highly highly recommend dark green and yellow gold nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iejyzcxabesc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1bverkf</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Loving the butterfly nails trend 🦋</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bverkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1bve6qr</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bve6qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1bvdhqg</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Nail shape :(</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvdhqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1bvdho0</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>🖤🖤🖤how’d I do for “goth glam” ? POLY GEL 💕</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvdho0</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1bvcjms</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Never had coffin before. Definitely in love.</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sua2kebodsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1bv7ab3</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Prebond vs. Foundation (Beetles)</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv7ab3</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1bvcd5r</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Look at how ridiculously flat my thumb nail grows out. It's like a Pringle 😵😅🤭</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d02w56xqmdsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1bvbo89</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opi nail envy milky for anyone else? </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wry7stwugdsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1bvblz8</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Favourite nail tips for smaller nail beds?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bvblz8/favourite_nail_tips_for_smaller_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1bvbikl</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Late to the pearl trend but I love em</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvbikl</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1bvb6gr</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Hate the length of my nails</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt561vtqcdsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1bvb6bq</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Builder gel lifting help please!</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu6ulyzocdsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1bvamuq</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>First time drawing Kuromi lol what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pix57x798dsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1bvaawj</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7t7yfhj5dsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1bva2c0</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Brush takes polish off?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bva2c0/brush_takes_polish_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1bv9v8z</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Removing Gel-X Extensions</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bv9v8z/removing_gelx_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1bv9v0q</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Short but fabulous nails</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58w7ooe12dsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1bv9nri</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>How do yall wear natural nails without having leftovers from darker nailpolish or have the topream yellow instead of white</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv9nri</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1bv9go9</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>These were harder than I thought to stick on!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv9go9</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1bv99j4</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Classic</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sczopn9xcsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1bv95rw</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Square or Different Shape?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krzsuodgwcsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1bv906y</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>I am NOT a professional by any means</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv906y</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1bv8zvy</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>🥴</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2iij9bu8vcsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1bv7nto</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Highly recommend getting whatever your inner 13 year old self would pick. So much fun!! </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/feoi3du7lcsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1bv7l9w</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>First Builder gel attempt. Feedback? 🫡🩷</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv7l9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1bv6qe5</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>💙💙</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocwbxw8eecsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1bv6c34</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Some nails I did :)</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv6c34</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1bv635y</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>My first fill and nail art! 🍒 🌼</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv635y</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1bv5ff8</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>First Time Doing Gel-X, took 5 hours. Looking for tips to improve!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv5ff8</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1bv5ewy</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Just a little sparkle this time 💖</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om2ubn435csc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1bv580u</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Besties New Nails</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owykqs4q3csc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1bv569x</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Newbie trying to discern quality</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv569x</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1bv4hev</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>First go at a gel gradient.</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iocd7cpmybsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1bv3y2z</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>What I do when I break a nail</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie8ucapzubsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1bv3xig</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>My 3 year old daughter told me they're "too much," and "maybe I can try new ones." Sadly she's not wrong 🙃</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g18jvemvubsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1bv3ptc</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>✨🖤</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv3ptc</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1bv3gqs</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>You know I gotta do the signature hand gesture now. First time doing full French Tips! All products are Light Elegance on natural nail length 🤍</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv3gqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1bv2xh7</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Are these due for an infill?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv2xh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1bv2vrh</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Glitter bow set by me 🎀</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdgjkw4mnbsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1bv2vo6</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Got these cuties after months of going without.</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1a74milnbsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1bv2054</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Mooncat’s Garden of Evil</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv2054</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1bv177j</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>🤎</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yytggc7cbsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1bv0p06</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>I love nail stickers but I hate that I always break this one nail (natural nails)</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpxbs07w8bsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1bv00n7</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Springy 🌪️🌸</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv00n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1buzfg8</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Manager let me have nails when I’m not supposed to :-)</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buzfg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1buzdq0</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude for work </t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1buzdq0/nude_for_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1buyu69</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Simple shapes on sheer background</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqdein1awasc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1buyoty</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>BIAB under gel-x? And removal question…</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1buyoty/biab_under_gelx_and_removal_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1buyoti</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Did this yesterday, I kinda like it</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96ezpfr1vasc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1buxsoq</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>🤎🤍</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmdz4gr9pasc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1bux3ha</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decided to treat myself </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eumz8udgkasc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1buwria</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Black Frenchies :p</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buwria</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1buw2zx</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Tiffany Blue!!!</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3k6y2xfdasc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1buvzso</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>I am in love😍😇🥰</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buvzso</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1buvpp1</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Some simple spring nails. Still growing them out, I find if I have no polish on them I go back to nail biting</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buvpp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1buvouw</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Milky lilac 💜</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buvouw</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1buv6n1</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Spring nails ❤️</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buv6n1</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1buu67w</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Started doing my own acrylics/dip nails 1 year ago here is my progress</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buu67w</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1burute</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>OPI Barefoot In Barcelona Dupe?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1burute/opi_barefoot_in_barcelona_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1buvbnr</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>🍓✨</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buvbnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1buudhc</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Some spring nails! 🌸</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b2bd8u81asc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1butjs6</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Lengthened my nails at the salon</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwvmyj0zu9sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1busskk</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Not sure if I’m being too picky here!</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1busskk</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1burcss</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>My spring nails!!</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1burcss</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1buqvbs</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just finished painting my Melanie Martinez nails 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cifkvpim89sc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1buq830</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Birthday nails ! I’ve never had stilettos before but I love them already</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buq830</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1buphdh</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Glitter gradient nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a436s7fou8sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1buottb</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Cracks in diy Nail dip</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1buottb/cracks_in_diy_nail_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1buo6fp</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Nails are breaking</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tr8xzomf8sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1bun7tu</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>blooming gel!</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mpgzbph38sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1buk4kc</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Help With New Nail Colour/Shape (Spoiled for Skin Condition)</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buk4kc</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1bvhama</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Colors by Llarowe “Black Gold, Texas Tea</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19ywg1t32fsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1bvcs0e</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>How do we feel about symmetrical skittles?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydjyq7xcqdsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1bv72gj</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Any suggestions for good peel of base coats</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bv72gj/any_suggestions_for_good_peel_of_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1bvcayx</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Bio oil?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bvcayx/bio_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1bvatoj</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Snow Cap</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvatoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1bva4pl</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>March Madness!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bva4pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1bva2cr</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Ready for spring 🌷</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muq308gm3dsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1bv92ca</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>velvet heart cat eye thing</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/t/ZPRTQfJqG/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1bv8lbt</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Sparkle sparkle</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv8lbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1bv6z84</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Grape soda by Color Dept.</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqiuvq07gcsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1bv3xc3</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Fake nail 101</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bv3xc3/fake_nail_101/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1bv54q9</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>My obsession with velvet nails is getting out of control</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv54q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1bv4k00</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Sparkles fix everything ✨</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6iqtpln1zbsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1bv46yj</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>A little splash of fabulous on my grief</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv46yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1bv3ye2</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>What are your favorite brands for pastels and neon pastels?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bv3ye2/what_are_your_favorite_brands_for_pastels_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1bv3tbk</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Dupe for Picture Polish Majesty?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydvr49t2ubsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1bv2u3v</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer has stolet my entire heart 👯‍♀️</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv2u3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1bv3lqp</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>You know I gotta do the signature hand gesture now. First time doing full French Tips! All products are Light Elegance on natural nail length 🤍</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv3lqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1bv1wyl</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Hot Girl Summer</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv1wyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1bv1g8b</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Anyone know how to achieve the blooming gel look on regular polish?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bv1g8b/anyone_know_how_to_achieve_the_blooming_gel_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1bv0f2r</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Is Moon Shine Mani any good?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bv0f2r/is_moon_shine_mani_any_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1buzk0o</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>A shifty polish + a thermal polish = ✨magic✨</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lryhkms71bsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1buwgrg</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>New Favourite Polish! (Phoenix Indie - Pelvic Sorcery)</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/021vd8zrfasc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1buyxwd</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Lullaby 💕</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buyxwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1buykm5</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Mooncat Skittle</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buykm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1buyfiq</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Good magnetic polishes to try out?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1buyfiq/good_magnetic_polishes_to_try_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1buydvr</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>calcifer 🔥</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buydvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1buxh2a</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>In search of...</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8taj0re1nasc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1buwxi2</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Mooncat “Hermit Crab”</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buwxi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1buwruv</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>So are we all wearing ILNP Eclipse for the eclipse on 4/8 or...</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1buwruv/so_are_we_all_wearing_ilnp_eclipse_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1buw1xa</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Tiffany Blue!!!</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1rsob38dasc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1buw10t</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Can someone share a dupe recommendation for the Cirque color "Lavender sky"?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1buw10t/can_someone_share_a_dupe_recommendation_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1buvsy0</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>sure, deceptive swatch photos are out there, but some polishes change drastically depending on lighting and angle!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buvsy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1buvidh</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Fucking wow.</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg2iwpjc9asc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1buv4g2</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>let my boyfriend pick this week’s color!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mna15bnl6asc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1buv00y</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Thanks to those who recommended I Scream Nail toppers!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1buv00y/thanks_to_those_who_recommended_i_scream_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1buuomy</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Written Invitation </t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bshyzqig3asc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1buuj4f</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Feeling sagely</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okkoph0c2asc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1buufnb</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>i live for the gloom &amp; doom. ⛈️💕✨</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buufnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1but93t</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>[M31] My wife does a great job on these🥰</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d95p45tqs9sc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1bus90a</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recs for jaw dropping royal blue polishes? </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sfh4fisk9sc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1bur1v5</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Do You Love the Color of the Sky?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bur1v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1bveqta</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Naughty &amp; Nice</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzzjyikr8esc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1bve4dv</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Retro spring vibesss✨💐</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oglbfluo2esc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1bve245</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Giving princess fairy vibes</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72ys2v032esc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1bvdwrv</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Golden but neutral</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vzmrulo0esc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1bvdeia</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>🖤🖤🖤how’d I do for “goth glam” ? POLY GEL 💕</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvdeia</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1bvd8dc</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfjll5kfudsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1bvcb5f</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>The cutest design I have done so far.</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icwvsby9mdsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1bvbkzs</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Pearl-y chrome nails I did on myself</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvbkzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1bvavvj</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Blue Eye Samurai</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvavvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1bv9nwa</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Spring 🌼 😊</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zesn0sbg0dsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1bv91vm</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>🥴</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ym4spbnvcsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1bv8aiw</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>New gel-x set 🥹</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv8aiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1bv1vyx</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Made these for the upcoming Eclipse 🌞🌘✨</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fhlvb4vgbsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1buy0sj</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Spring set but make it creepy 💀</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buy0sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1buxzih</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>pretty in pink 🎀ིྀ</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buxzih</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1buof0b</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>70’s vibes? 🌻</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1buof0b</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Apr  5 08:08:07 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_07.xlsx
+++ b/data/2024_04_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C735"/>
+  <dimension ref="A1:C860"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12928,6 +12928,2131 @@
         </is>
       </c>
     </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1bwccp2</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the pleasure of having neat and painted nails and with shine better </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ttsnqme9msc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1bwcb40</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Matte Pastels</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwcb40</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1bwa60f</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spring Vibes </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrpd99rjjlsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1bw9of5</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Finally got my nails done</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg9obsoqelsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1bw8ukn</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Does buffing a gel-x tip before painting really help the paint stick better?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bw8ukn/does_buffing_a_gelx_tip_before_painting_really/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1bw87u6</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>I love that they are growing on me 😍</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lqjeah91lsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1bw7oi8</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Am I due for a fill? (Newbie)</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw7oi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1bw71pl</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Thin destroyed nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bw71pl/thin_destroyed_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1bw1au2</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Help with cracking or splitting</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw1au2</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1bvz64l</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Inspo </t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dtzqc634jsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1bw5h9h</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>In love</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8s5djif4eksc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1bw59cm</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>I hate Kiara Sky polish</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bw59cm/i_hate_kiara_sky_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1bw59bp</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>🌈 🌈</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw59bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1bw3u08</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>New set 💗</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw3u08</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1bw3s4s</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Winnie the Pooh nails</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw3s4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1bw3kzu</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Blue💙</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kn28leezjsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1bw2ajy</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I think I went overboard with my sping nails.. lol.</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw2ajy</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1bw28qy</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>A little more obnoxious than I anticipated lol</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw28qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1bw0exm</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Purple Mani</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hfvqhudcjsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1bw0e7h</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Builder Gel</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bw0e7h/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1bw0at0</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Glossy or matte? Chocolate…with some gold🍫⭐️</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw0at0</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1bvys69</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Pink and glitter for recovering peeling nails ♡</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvys69</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1bvxw5l</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I can’t wait for summer! Especially when clients want me to do nail art like this</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6wxc2sivisc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1bvw3g4</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Tragic loss today</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvw3g4</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1bvvesy</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Cherry Blossom season 🌸</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/117gpsyyeisc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1bvv45t</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Feeling blue</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dowczw01disc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1bvuhak</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Easter mixed with some Spring Fling Nails</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au0yhboo8isc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1bvu6xe</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Trying to grow out my natural nails again 💜</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvu6xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1bvtt0y</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Builder gel first timer</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvtt0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1bvspdx</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Still have to clean the edges, but I’m obsessed 💜 [details in comments]</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvqzq1wcwhsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1bvrq72</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Nails keep lifting</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqem7epiphsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1bvsirg</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Color underneath is my new favorite thing</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5g0py9z4vhsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1bvsbsv</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Green? For spring? Groundbreaking. ☘️</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzi3354tthsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1bvrv8n</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>This color 😍</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssrs9d0lqhsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1bvr0qg</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Ready for summer</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt873dflkhsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1bvr0go</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Spring nails🌼🌱🌾🍄🪺</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvr0go</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1bvq2nx</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My second French attempt!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zrryzjvdhsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1bvq034</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Just wanted to share a few of my favorite sets from the last few months! I love my tech so much</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvq034</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1bvpz59</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>I tried squoval, does it suit? Usually get almond ♥️</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0gnj2badhsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1bvovcs</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvovcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1bvod5f</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>what do we think?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qnj6e5y1hsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1bvnsjb</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>birthday nails !</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvnsjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1bvnhr0</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Where to buy good gel</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bvnhr0/where_to_buy_good_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1bvn6nt</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Graffiti serie - part 2</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvn6nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1bvn363</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feels like spring </t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/teccfb17sgsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1bvn23n</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>I really love my current nail colors</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2al47ckxrgsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1bvlqea</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>First time getting pink &amp; white! It’s my natural nails under the gel 🥰</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fdmoe6mggsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1bvlkx6</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Got Nails done at the Salon, design based on Nat de Nail's art on Youtube</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvlkx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1bvlg8a</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>First time with acrylics!</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvlg8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1bvl2wy</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Just tried a new art, your thoughts?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylbmnardagsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1bvjv9v</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Fairytale Nails 🍄🌿</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvjv9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1bvj95n</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Back to purple</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phfg1z7mqfsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1bviqlc</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>🐝&amp;🐞</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bviqlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1bvip99</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>My April set</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvip99</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1bvafle</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Painting normal nail polish over gel?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bvafle/painting_normal_nail_polish_over_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1bvds9f</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Why are my pinkies so different?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvds9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1bvhrqu</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Matte finish is underrated IMO!</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvhrqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1bwbh09</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>😞</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvrcbk0gylsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1bw92kv</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Last time I broke a nail I put a sad face on it; this time I wanted to be a little more positive</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw92kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1bw7920</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Recommended shape for my nails? I used to be almond, I went squoval for a little.</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw7920</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1bw782g</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>recs for shades from these brands?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bw782g/recs_for_shades_from_these_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1bw5yh4</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Earthy Spring 🌱</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw5yh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1bw5y0g</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Me tonight… RIP nails 😭</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrleboouhksc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1bw508q</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Mooncat- Monster under your head</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oyj1vf0eaksc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1bw43ox</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Is it risky to use cheap gels on fake nails?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bw43ox/is_it_risky_to_use_cheap_gels_on_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1bw39f6</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Lucky 13 - And in the Mornin I'm Makin Waffles</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw39f6</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1bw2xh3</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Revved Up Like a Douche</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw2xh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1bw2wyd</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Tradie Lady</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw2wyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1bw2tsx</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Gelly Look manicure</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj8w6v1ntjsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1bw1j59</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>I think I love thermals ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1iywz4bkjsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1bw1i05</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>OPI Repair Mode Vs CND Repair Rxx</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bw1i05/opi_repair_mode_vs_cnd_repair_rxx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1bw167e</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Swatch time🍫</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw167e</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1bw10xq</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>I thought I had food stuck to my nail but turns out it was broken 💔💔💔</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw10xq</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1bw0nsd</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Y’all be sleeping on Shleee Polish</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw0nsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1bw0n0t</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Help finding a dupe</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzpegwhydjsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1bw0mbu</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Need help on how to get better nails</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw0mbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1bw0m93</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Opal Powder top coat issues</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bw0m93/opal_powder_top_coat_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1bvzws8</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Polishes with Angry Sounding Names</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bvzws8/polishes_with_angry_sounding_names/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1bvymlx</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Does this color suit me?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxjjg4xh0jsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1bvuqxm</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>How can I fix my nails?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvuqxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1bvxsk0</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Mushroom nail art 🍄</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvxsk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1bvxiod</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Spring time nails - love the little daisies!</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvxiod</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1bvx8k0</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>If you could only have 15 polishes</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bvx8k0/if_you_could_only_have_15_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1bvvple</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>I’m obsessed 😍</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnohm51zgisc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1bvvl4z</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Violet Large Particle Topper?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bvvl4z/violet_large_particle_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1bvux50</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>New Favourite Green</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvux50</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1bvuk17</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>New stuff :)</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9f989k79isc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1bvtxw8</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Cirque Blue Velvet + Horseshoe Magnet</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3wh8spz05isc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1bvtuwo</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Getting used to gel! I think this is my 5th time.</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvtuwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1bvsv00</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>2019 PPU Beauty</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nho4u6jfxhsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1bvrocv</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Happy I stepped outside my usual colors</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvrocv</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1bvshu7</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Tomato fiesta on the inside, and snow on the outside. Let’s put these thermals to work!</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvshu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1bvrlku</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI gel -- what colors to avoid? Some seem to be too thick? </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bvrlku/opi_gel_what_colors_to_avoid_some_seem_to_be_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1bvrc1i</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Last week's easter skittle mani! Inspired by the copious amounts of Cadbury eggs consumed over the past week.</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1g0rdnhsmhsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1bvqo1f</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Speckled spring nails</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvqo1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1bvpygh</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Late Easter nails</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvpygh</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1bvpwos</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>When painting swatches, do you use a base coat?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jmgqsftchsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1bvp57o</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>For those of you wanting to see Indomitable with a matte finish</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxsfl21h7hsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1bvnztm</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Brick red flakey</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/VDYy12h</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1bvnnnm</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Recommendations for adhesive press on tabs?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bvnnnm/recommendations_for_adhesive_press_on_tabs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1bvnl41</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Fun with Spring shimmers!</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gvl9lp2tvgsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1bvn9wk</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Blooming Azalea</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvn9wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1bvmhsw</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>mooncat sale?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bvmhsw/mooncat_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1bvl9lk</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Secrets To Keep - EDM 💙</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3755mndcgsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1bvkq4x</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>La Lune</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvkq4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1bvkesj</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Nail hardender</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bvkesj/nail_hardender/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1bv77si</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Inspired by Phoenix Ivy</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bv77si</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1bwccn8</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Nail marble attempt</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwccn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1bwag7o</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Hello kitty!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ip0bnzqjmlsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1bwa0nu</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Lavender bloom 🪻</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwa0nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1bw5p76</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Love this set but want to try another color instead of green(keep everything else as is). What other color would it look good in?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw5p76</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1bw3bsm</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Recent sets I’ve done😍</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw3bsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1bw30p2</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>A gem 💎</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ridxs542vjsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1bw2o3q</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Lisa frank vibes✨💖</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbd8eg6hsjsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1bw2bq4</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Stained glass tulips!🌷</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lajkx381qjsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1bw26md</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>An attempt was made.</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvho306zojsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1bw00ev</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>BINGO</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bw00ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1bvzkpf</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>I’m spam posting my nails 🤣 but this cutie set of Halloween nails I made as a beginner 👻</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r03vdpcu6jsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1bvxm44</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Copying creepy spring nails</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvxm44</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1bvv00v</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Birthday nails 🍒</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvv00v</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1bvt6gh</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>My aunt let me practice on her nails 🖤</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e06sp0dozhsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1bvqi06</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Like? </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94w6ij5yghsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1bvox7q</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvox7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1bvndkc</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Graffiti serie - part 2</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvndkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1bvhuud</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Matte finish looks so fine if done right!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bvhuud</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Apr  6 08:07:00 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_07.xlsx
+++ b/data/2024_04_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C860"/>
+  <dimension ref="A1:C998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15053,6 +15053,2352 @@
         </is>
       </c>
     </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1bx67r1</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Very simple but took me 5 hours</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx67r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1bx66wy</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Got these yesterday and they are so damn shiny in the sun</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qxyku273gtsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1bx62yf</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spring Thistles </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b9gbglvetsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1bx4m08</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>How do I start painting my dominant hand?</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bx4m08/how_do_i_start_painting_my_dominant_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1bx5bbv</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Cuticle Area Application</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx5bbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1bx4bmt</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Anything I can do to tone these gel-x nails down?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx4bmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1bx2noo</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nails! Any tips? </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixjqhtvmdssc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1bx2i1d</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite set so far (Spider-Man and Symboite) </t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0j5gyv4cssc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1bwxcfc</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Difference between russian manicure, dip, and acrylic tips?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwxcfc/difference_between_russian_manicure_dip_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1bwy6y0</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Ski jump nails</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwy6y0</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1bwt4sf</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>First attempt at 3D, and Blooming Gel.</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwt4sf</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1bwsiql</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Cosmic Brownie nails inspired by Morakava’s chocolate nails ❤️</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwsiql</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1bwkieh</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>New Nails!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwkieh</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1bwonm2</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>The matte and gloss tips update🍫😎</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcpmm15capsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1bx10s8</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Don’t mind how eh my hands are but these are some of my favourites</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx10s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1bwzy0t</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>I love these</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc2qn39morsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1bwzqfy</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Super basic but I tried press ons for the first time and I’m well pleased</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwoe436smrsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1bwzp41</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Red is my favorite.</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwzp41</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1bwz9pm</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Butterfly nails !</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwz9pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1bwyx5n</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Noob here with nail question </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwyx5n/noob_here_with_nail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1bwyrq0</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Boston Nail Techs?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwyrq0/boston_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1bwybaq</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Some of my absolute favorite sets from the past year!</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwybaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1bwxuh1</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polygel nails lifting </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwxuh1/polygel_nails_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1bwxu9x</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>minimalistic pink design 🌸🎀🩷</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwxu9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1bwx555</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Are these as bad as I think they are?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwx555</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1bwx3ka</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>DND unicorn lovely with sparkles on top</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qx5h7z9g0rsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1bwwov0</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Treated myself to some spring nails 💅</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwwov0</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1bwwiwf</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>His and Hers Mani</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwwiwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1bwwfr0</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>1st Russian Mani</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwwfr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1bww63w</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Tried out the butterfly trend 🦋</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e00b6r34tqsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1bww3rj</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Retro vibe?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmhpyk6nsqsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1bwvus3</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Pastel skies ☁️</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbpfp29uqqsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1bwv4ln</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>The perfect teal 🩵💅🏼</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ek0uxpahlqsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1bwuiuv</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>My natural sharp claws</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqdzj4f6hqsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1bwto82</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Ohora N Snatched</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwto82</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1bwte5w</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Beginner at-home gel nail recommendations</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwte5w/beginner_athome_gel_nail_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1bwsofc</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Neon Duo for New Orleans</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ift9bjn34qsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1bwsmzb</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>absolutely IN LOVE with these french tips.</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwsmzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1bwshim</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>are there any wide nail bed friendly press ons/nail tips?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwshim/are_there_any_wide_nail_bed_friendly_press/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1bwshfb</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Finally made the jump into summer colours! 🧡🩷 only realised that they match my bracelet after taking this pic🤣</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzpgdh9n2qsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1bwrsd4</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Stain-glass Stilettos</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t14smhmkxpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1bwri1m</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Sanrio nails</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwri1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1bwr6t1</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>A very fun spring set 🐸</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itt1i506tpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1bwr11y</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Gel Nails Growth after 4 Weeks</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwr11y</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1bwqtjh</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there anything I can put on my nails that is natural for strengthening etc? </t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwqtjh/is_there_anything_i_can_put_on_my_nails_that_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1bwqsxt</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Nail Types and Events</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwqsxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1bwqmjn</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwqmjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1bwql1t</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7goqaxhnopsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1bwq7h9</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>The update #2🍫🥰</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p4x4udslpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1bwq1yj</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Sea foam green nails! Tried something new. Does it look okay? I am trying to grow out my nails.</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe4dkbaokpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1bwpwt3</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>My attempt at tortishell nails. I don’t hate em but I don’t love em lol critiques welcome 🤗 (ss from vids in diff lighting cause reddit camera quality sucks)</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwpwt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1bwpoo9</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>First time trying Bio gels</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o17c4a0whpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1bwpmaz</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Aura nails! ✨🤩</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwpmaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1bwo9sn</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>got new color 🩷</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elqcsbuj7psc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1bwo952</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Buffing nails </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwo952/buffing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1bwmy3w</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Black nail art 🖤🔥</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwmy3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1bwmpgl</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>gouache paint for nail art?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwmpgl/gouache_paint_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1bwm5oc</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>minty fresh new spring set 🍃</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyzvzek2sosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1bwlrvh</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Dip Powder Recs</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwlrvh/dip_powder_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1bwll67</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwll67</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1bwlh7q</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Ohora Nail Strips</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unkp1vc5nosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1bwleuj</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Bagels and lox nails 💅 🥯</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwleuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1bwk4ly</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Easter Nails </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9o5dc8nadosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1bwkc9l</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Should I keep going</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y48ikphueosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1bwh78e</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>New builder gel. is this normal?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/drmrjbihqnsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1bwf3he</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Dip Nail Sets</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwf3he/dip_nail_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1bwjh6g</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Nails lifting after doing the dishes</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bwjh6g/nails_lifting_after_doing_the_dishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1bwizfd</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>My nails I had for Greece, everyone there loved them 🇬🇷(also got engaged while there!)</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86exrurq4osc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1bwi8cc</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>2 problems with acrylics</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ky2nf0zynsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1bwgz49</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Did my sisters nails today!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwgz49</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1bwgct1</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>A recent acrylic set I did</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwgct1</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1bwez2h</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Skittle love 💜💅</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67mncjew4nsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1bwev46</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Trying this again</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yeatttfo3nsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1bwer1x</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>cherry blossom colored nails</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcc05wsd2nsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1bwei1f</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Some art and a curve. &lt;3</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwei1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1bwdtty</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Ridges on Nails</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwdtty</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1bwdoyx</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>pastel yellow chrome mani</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwdoyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1bx446x</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Any non-gel milky/jelly white polishes?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bx446x/any_nongel_milkyjelly_white_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1bx2xvu</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>I’ve been manifesting this color!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx2xvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1bx07ti</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Hard gel Nails!!!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx07ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1bwzx6p</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Peely base.</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nz19siforsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1bwzo8g</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make this stop? </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyds61w8mrsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1bwznae</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>3 days later.. sally hansen gel miracle already chipping and peeled off on my thumbs and index finger lol (repair rescue base and revlon top coat)</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwznae</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1bwzkuk</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Dead Tired</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwzkuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1bwzkpa</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Natural nails new ig page</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwzkpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1bwym0m</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>What Dreams Are Made Of</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wtr8ptizcrsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1bwxd2s</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>i'm blue dabadidabadie 💙🌀🧊💧</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwxd2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1bwxb9m</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>There you are, sweetheart.💗💜💙</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40pleyi82rsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1bwx810</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Y’all made me buy it</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwx810</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1bwvzwr</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Another glowy mani</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06s276qtrqsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1bwvxub</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Getting impatient waiting on my nails to grow, thought my nails should match my mood</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo6i7qzgrqsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1bwuzde</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Blue Lagoon Jelly</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lirbtwgkqsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1bwubb4</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Removers and Acetone additive questions</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bwubb4/removers_and_acetone_additive_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1bwsog2</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>New bees knees collection is too beautiful</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wicfvl044qsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1bwsgq8</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>I think I've found my favorite nude</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au9gg9n42qsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1bwrobd</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Lucky</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2iijhnqwpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1bwrhdt</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Exhibit A as to why I’m a diehard 3 coat girlie 💚☘️ </t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wy5orwbvpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1bwqvft</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Bouquet Toss - Natural vs Flash</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwqvft</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1bwqgiu</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Kbshimmer's Amanita Moment</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urbozd7pnpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1bwqb97</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>A Subtle Thermal🌡️</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwqb97</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1bwprm6</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink tips 💗 </t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlsw0egiipsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1bwp281</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Nail polish too streaky?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwp281</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1bwol82</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Some Ethereal and Lumen Swatches</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwol82</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1bwnvuq</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>It definitely pulls more coral irl but it’s still a very pretty spring polish!</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79jnw0xo4psc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1bwmsij</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🎵  Hey now, hey now 🎶 </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h54m7cynwosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1bwmkwi</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>is something wrong with this top coat?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwmkwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1bwm5uj</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>So many colors! Alchemy Lacquers - Dusk Hallucination</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwm5uj</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1bwlvkl</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>ILNP Celeste is unexpectedly good</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwlvkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1bwla8t</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Sea-ing is believing!!!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwla8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1bwl2do</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>BAM! 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwl2do</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1bwl1i3</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Cirque Marsala Jelly chipping much faster than my other polishes</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bwl1i3/cirque_marsala_jelly_chipping_much_faster_than_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1bwkwhg</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>ILNP Sleigh Bells</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwkwhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1bwkqy3</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>ILNP Pool party</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwkqy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1bwkpl0</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Why is my nail polish "cracking" while it still feels smooth if I run my finger over it?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyj3k5lfhosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1bwkm5k</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>{PR} All the shifty/glowy is all I want 🤓</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxw1z0yugosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1bwke34</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Experimenting with Fairy Dust as a topper</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwke34</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1bwk6f1</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Nausicaä: Poison Spore by Nailed It!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtmhvexodosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1bwjpuf</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>How long is long enough? 🤣</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7totg19aosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1bwjbwi</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Trying to shoe off the shift...</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwjbwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1bwi9vb</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>ILNP Thick/Goopy?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bwi9vb/ilnp_thickgoopy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1bwi041</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>This polish really is incredible! I've had it on for 5 days with no visible wear at all! My first photo was day 1, 2nd photo is today.</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwi041</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1bwhbtu</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Finally trying this one!</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ea8k573mrnsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1bwh5j5</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>How many polishes do helmers hold?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bwh5j5/how_many_polishes_do_helmers_hold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1bwgyb8</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>This is a very dumb question, but does ILNP dry with a UV light?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bwgyb8/this_is_a_very_dumb_question_but_does_ilnp_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1bwgpm9</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Tfw when wake up and suddenly remember your nails are hot pink today 🔥</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iy2mddx4mnsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1bweuyu</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Skittle love 💜💅</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d2l808m3nsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1bwyke7</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Sunny skies! ☀️🌈</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwyke7</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1bwrrn0</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Koi fish nails🫧</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ph8lum9dxpsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1bwrim9</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Spring nails 🌿🌸</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwrim9</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1bwrfmw</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>One of my favorite ombré set on short square😍</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zowlikcyupsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1bwpxqp</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>My attempt at tortishell nails. I don’t hate em but I don’t love em lol critiques welcome 🤗 (ss from vids in diff lighting cause reddit camera quality sucks)</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwpxqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1bwpi0o</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Aura nails! ✨🤩</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwpi0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1bwnwj5</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>What you think about my design? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtoaz0cu4psc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1bwm19r</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>This time I opted for a pastel color, what do you think?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93zw5nm6rosc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1bwkvn0</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Plant inspired new Nail Look 🌱</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwkvn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1bwke8m</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Bagels &amp; lox nails 🥯 🐠 💅</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwke8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1bwfmyi</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Spy family!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1xvnufxbnsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1bwdoru</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Advices?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bwdoru</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Apr  7 08:09:15 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_07.xlsx
+++ b/data/2024_04_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C998"/>
+  <dimension ref="A1:C1144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17399,6 +17399,2488 @@
         </is>
       </c>
     </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1bxz3qn</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Just a pink mixed manicure theme</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxz3qn/just_a_pink_mixed_manicure_theme/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1bxyp0d</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Week 3 of Making Pressons Everyday</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxyp0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1bxymt0</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Spring Pedicure</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmxxb7lag0tc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1bxyjze</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>acrylic nails fill</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxyjze/acrylic_nails_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1bxxq41</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Brown French</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxxq41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1bxxnio</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Spiced up my nude a bit.</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxxnio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1bxxhv7</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>First builder gel set with tips</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxxhv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1bxxcun</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxxcun/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1bxx8fe</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5z7d9xk00tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1bxx1d9</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Is there a secret trick with how to put on glitter nail polish?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxx1d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1bxwind</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>I fcked up</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxwind</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1bxvyo9</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>These took me way too long ✨</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qbvs1a1nzsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1bxvn3z</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Pink french Chrome combo</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5xpp45sjzsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1bxrh0v</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>New to the world of nails</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7l756zmhysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1bxqyp1</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>What brand of sticky tabs are the strongest for press on nails?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxqyp1/what_brand_of_sticky_tabs_are_the_strongest_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1bxpxyx</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>i tried out nuanced nails !🪷🌷</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/14aj57cu4ysc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1bxucnf</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Some fun cat eye nails!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxucnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1bxtifq</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>💟</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr5d74bqzysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1bxt1r4</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Good Spring Color?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxt1r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1bxsmpm</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Does anyone still get regular manicures from a nail salon?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxsmpm/does_anyone_still_get_regular_manicures_from_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1bxslmg</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Little spring blossoms 🌸</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxslmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1bxr6ho</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Obsessed with this lilac glitter combo</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/az2lj4a5fysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1bxqcjs</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Flowers!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnv24hr48ysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1bxqb2a</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails peel when I clip them </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxqb2a/nails_peel_when_i_clip_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1bxq78w</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Is it very obvious that these are stick-on nails (in a negative way) I can't tell</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxq78w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1bxpu0m</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Thermal polish ✨️</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxpu0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1bxo1a6</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Pretty new to doing my own nails, but this is probably my favorite set I’ve done</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7kga04tpxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1bxnucb</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Help! How do l fix this?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i68qqdlcoxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1bxp5g1</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>RUSSIAN MANICURE</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxp5g1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1bxfqe1</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Graffiti serie-part 3</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxfqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1bxd6n8</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>polygel 🐌🩷</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxd6n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1bxox35</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zen Garden nails 🌸 </t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ek0aoyowxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1bxov8u</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>My nails done by a technician vs done by me lol got me looking all green lol</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iikjr6icwxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1bxoho7</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Marble Nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw2qd7getxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1bxobzp</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Changing nail shape</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9qhbnn5sxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1bxoaxb</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>I found a new salon 😊</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxoaxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1bxnush</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Nail salons across the UK to collectively raise prices</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/av/uk-wales-68740412</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1bxngtt</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Simple but totally in love with them</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fy3qv22glxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1bxneop</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Seafoam Green</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxmtgc5zkxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1bxm227</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>In love with this set</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6t93t8claxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1bxlqk5</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Third Set of Press Ons</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxzsqn378xsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1bxldiv</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Two coats of Sinful Nails base coat did nothing to prevent the following Zoya Erza from staining my nails. What is your favorite base coat to prevent staining? </t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9cubwof5xsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1bxkrth</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Shrooms for spring 🍄</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnn8a5sv0xsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1bxkl91</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>nails to match my bag</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxkl91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1bxkb5g</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>One of my favorite sets!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxkb5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1bxjtq6</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Shape advice</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g18t8jgttwsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1bxjoid</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>This polish under the flash looks fucking amazing! 📸</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxjoid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1bxjkoq</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>🦋🦋</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25vyocexrwsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1bxjibq</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Simple nails with evil eye design</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxjibq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1bxj5dr</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Sheer pink 💗</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxj5dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1bxj5d8</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Some flower nails to welcome the spring season!</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3folsc1powsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1bxj4ax</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Nails constantly look dirty...</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxj4ax/nails_constantly_look_dirty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1bxir0o</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>my first acrylic nails I love them so much</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxir0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1bxionp</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Cleaning sugar glitter nails?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwd433a5lwsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1bxfqde</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Protein bond for press-on nails?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxfqde/protein_bond_for_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1bxf72f</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>My nail lady did not have to go this hard</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxf72f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1bxepfc</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Any advice/tips on how to apply this type of glitter?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j31ffqq8rvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1bxejri</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>My nails for our vacation to Japan during cherry blossom season!</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gza1tovzpvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1bxegtd</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>raindrop nails</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxegtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1bxe9x8</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>yall think the blue is cute or not?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5lcldawnvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1bxe0mq</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>New Color!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jj7z90cvlvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1bxcwt8</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Got my first ombre set today! I love them 💙</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbmnva26dvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1bxcrxi</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Mixed in a loose glitter with polygel for this french tip set</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxcrxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1bxcfrk</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Which gel polish brand on Amazon is a good one to start with? Want a mid priced option if possible, but a good brand to try. Any information is helpful thank you 🌼</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bxcfrk/which_gel_polish_brand_on_amazon_is_a_good_one_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1bxbdd9</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I chooped it unevenly </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6kfejsn0vsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1bx9k30</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>I'm so in love with my new set 😍👽🛸</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx9k30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1bx9glo</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Y2K chunky charm nails!!! </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upkfl71uiusc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1bx7h6c</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>New set (from a week ago)</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7n9vzg9qvtsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1bx7ae8</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Cute nails～</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17p2rj6gttsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1bx786w</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>The Magic of Nail wraps</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6sr9u8pstsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1bx71y8</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Press on nails made by me 🍓🍫</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4m31ctwnqtsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1bxyqmf</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Soft gel ‘press ons’</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bxyqmf/soft_gel_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1bxvw89</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Share your innovative techniques for blending the nail line &amp; nail bed under sheers &amp; jellies ⤵️</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bxvw89/share_your_innovative_techniques_for_blending_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1bxuy32</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eclipsing Eclipse </t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/we2froo1dzsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1bxuqvs</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Was craving a sparkly manicure</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghlrt8e4bzsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1bxu2xj</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Found a hack for too sheer polishes..</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxu2xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1bxtl70</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Habit - Jolly Bean Green</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvrkaaaf0zsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1bxtdi1</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Zoya Stevie with topcoat</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxtdi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1bxtb2o</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Update on polishes I packed for my trip</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkbn54gvxysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1bxsmmp</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Any recommendations for something similar to this?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otozl3yrrysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1bxsbhl</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>"I'm not good at art but, I can do a clean mani" abstract eclipse nails</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxsbhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1bxs9xn</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Favorite PEARLY whites?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8aw0w1noysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1bxrfbb</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>My first indie polish looks</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxrfbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1bxrf6j</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Melting ice cremes</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qlj7uk6hysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1bxqzqg</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Some love for ILNP Ava (plus mooncat base and essie speed setter)</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxqzqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1bxqo86</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>I heard we’re doing eclipse nails</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ig5ccxcsaysc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1bxqn2v</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Idk why I love this color so much</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxqn2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1bxq5pz</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>new diamond candles. 💎</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxq5pz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1bxq166</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Mooncat Winds of Fate</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxq166</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1bxpxuk</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Trying out new thermal polish ✨️</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxpxuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1bxot0p</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Broken Nail ⚰️💀🥀😐</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxot0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1bxodbs</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Obsessed with this glitter!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxodbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1bxnofz</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>INLP birthday suit is so pretty in the sun! ☀️✨</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxnofz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1bxnhsz</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Finally getting over my Stamping block 😈 🔥</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxnhsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1bxn1sb</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Things You've Learned?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bxn1sb/things_youve_learned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1bxmpuq</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Lynbdesigns Cat's Paw 💚💕</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxmpuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1bxmoti</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Thermals really light up my fife</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxmoti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1bxmbet</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Gel manicure - is this normal?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bxmbet/gel_manicure_is_this_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1bxm63z</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Ready for the solar eclipse! 🌕</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxm63z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1bxm22w</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Room For A Thousand</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30r68whlaxsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1bxlsu4</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Red is a classic for a reason (1st picture in natural light, 2nd picture in lamp light)</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxlsu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1bxk8wj</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>My husband chose this for me!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxk8wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1bxk4sn</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Has anyone else received broken mooncat polishes lately?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxk4sn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1bxjfq6</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Low effort Total Eclipse of the Heart manicure...</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgkp8cjuqwsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1bxj7dx</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>I have been crying out to you from the start -BKL</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qrr8ddx1pwsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1bxj2pv</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Kiss in the Wind</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxj2pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1bxik3n</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Thermals &lt;3</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxik3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1bxi4my</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Beach Cruiser Dupe</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bxi4my/beach_cruiser_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1bxi2hl</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Mystery tool! What the heck is this</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxi2hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1bxhvrm</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Lumen ‘Morpho Glow’</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxhvrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1bxh3vc</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Matching my nails to my lil snake today</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxh3vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1bxh2uh</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Me wondering why I love shifty shimmers and multi-chromes so dang much…</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39sfsbh79wsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1bxglf7</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Lumen - Morpho Glow</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p6hms3l75wsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1bxgjpu</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>too many ideas</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bxgjpu/too_many_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1bxftco</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Is there a such thing as clearcoat ridge filler that does basecoat as well? In quick dry?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxftco</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1bxfgqb</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Purple is purple-ing 💜</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxfgqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1bxfaic</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Cirque Colors, Madder</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/juruw6vovvsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1bxez7i</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Excuse the messy mani just testing a new shade I made, like it?</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxez7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1bxeo0k</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Fall Fire</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tgik16vmqvsc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1bxen97</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Do you like orange polish?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxen97</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1bxehxk</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Obsessed with Bees Knees 😩</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxehxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1bxeh2m</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>I wore only green polish during March</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxeh2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1bxdoep</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Y’all weren’t kidding about LynB Designs! ✨</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45v1fzx9jvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1bxdnoo</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not usually a fan of milky nails but some shimmer fixes that </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zq36w673jvsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1bxczu8</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Just the juiciest colors</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxczu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1bxchw0</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eclipse &amp; Eclipse for the Eclipse </t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0e1koy4x9vsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1bxbm4e</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>When you find out part of your polish is UV reactive</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2xeflen2vsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1bx4lg0</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Male pedicure with polish</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx4lg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1bx9ynw</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Phoenix - Chibi Chibi</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx9ynw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1bx8u07</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>For how long do you wear your mani?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bx8u07/for_how_long_do_you_wear_your_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1bx6wzw</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thinner for HT peely base and other QDTC/ base coat </t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/on9wrv20ptsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1bxutyt</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I declare this THE summer set(made by myself)</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s33ai19ybzsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1bxsm4y</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Spring Blossoms 🌸</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxsm4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1bxn096</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green eyed monster </t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t2xfr7uhxsc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1bxln57</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>What your favorite shape?IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lhi76zg7xsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1bxl9d0</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Creating Nail art makes me happy.</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxl9d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1bxkb6f</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Just finished making these press ons!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxkb6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1bxgcky</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Classy set IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/487v7keq3wsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1bxft4p</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Graffiti serie -part 3</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxft4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1bxffdv</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>What do you think of these nails? I used neon pink and neon yellow, put a base of clear first, marbled, cured, sanded, then added two more layers of marbling- I also dropped clear on top of the colors to create depth-</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nrdzgcqwvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1bxf3ib</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Pompompurin 🌟</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ifguvj6uvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1bxe6qb</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Not too bad for my Non-Dominant hand 💙🤍</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iklygvc6nvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1bxdvzi</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Fun Set IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tavp614vkvsc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1bxcvk3</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Did my friends gel x nails yesterday</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxcvk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1bxcqlv</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Mixed in a loose glitter with polygel for this french tip set</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bxcqlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1bx6ae7</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Ombre is GOATED frfr</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bx6ae7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>